<commit_message>
updated code for 8 sensors
</commit_message>
<xml_diff>
--- a/State_Cases.xlsx
+++ b/State_Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Case</t>
   </si>
@@ -32,15 +32,6 @@
     <t>Left Wall</t>
   </si>
   <si>
-    <t>Left Corner 2</t>
-  </si>
-  <si>
-    <t>Left Corner 3</t>
-  </si>
-  <si>
-    <t>Left Corner 4</t>
-  </si>
-  <si>
     <t>Front Wall</t>
   </si>
   <si>
@@ -50,52 +41,118 @@
     <t>Front Corner 2</t>
   </si>
   <si>
-    <t>Right Corner 1</t>
-  </si>
-  <si>
-    <t>Right Corner 2</t>
-  </si>
-  <si>
-    <t>Right Corner 3</t>
-  </si>
-  <si>
-    <t>Right Corner 4</t>
-  </si>
-  <si>
     <t>Right Wall</t>
   </si>
   <si>
-    <t>01100</t>
-  </si>
-  <si>
-    <t>00100</t>
-  </si>
-  <si>
-    <t>01010</t>
-  </si>
-  <si>
-    <t>01110</t>
-  </si>
-  <si>
-    <t>00111</t>
-  </si>
-  <si>
-    <t>00011</t>
-  </si>
-  <si>
-    <t>00101</t>
-  </si>
-  <si>
-    <t>00110</t>
-  </si>
-  <si>
-    <t>00001</t>
-  </si>
-  <si>
-    <t>Left Corner 1</t>
-  </si>
-  <si>
     <t>States - (left wall, front left corner, front, front right corner, right wall)</t>
+  </si>
+  <si>
+    <t>01100000</t>
+  </si>
+  <si>
+    <t>00100000</t>
+  </si>
+  <si>
+    <t>01010000</t>
+  </si>
+  <si>
+    <t>01110000</t>
+  </si>
+  <si>
+    <t>00111000</t>
+  </si>
+  <si>
+    <t>00011000</t>
+  </si>
+  <si>
+    <t>00101000</t>
+  </si>
+  <si>
+    <t>00110000</t>
+  </si>
+  <si>
+    <t>00001000</t>
+  </si>
+  <si>
+    <t>Left  F Corner 1</t>
+  </si>
+  <si>
+    <t>Left F Corner 2</t>
+  </si>
+  <si>
+    <t>Left F Corner 3</t>
+  </si>
+  <si>
+    <t>Left F Corner 4</t>
+  </si>
+  <si>
+    <t>Right F Corner 1</t>
+  </si>
+  <si>
+    <t>Right F Corner 2</t>
+  </si>
+  <si>
+    <t>Right F Corner 3</t>
+  </si>
+  <si>
+    <t>Right F Corner 4</t>
+  </si>
+  <si>
+    <t>Right R Corner 1</t>
+  </si>
+  <si>
+    <t>00001110</t>
+  </si>
+  <si>
+    <t>00001100</t>
+  </si>
+  <si>
+    <t>00000110</t>
+  </si>
+  <si>
+    <t>00001010</t>
+  </si>
+  <si>
+    <t>Right R Corner 2</t>
+  </si>
+  <si>
+    <t>Right R Corner 3</t>
+  </si>
+  <si>
+    <t>Right R Corner 4</t>
+  </si>
+  <si>
+    <t>Rear Corner 1</t>
+  </si>
+  <si>
+    <t>00000111</t>
+  </si>
+  <si>
+    <t>00000101</t>
+  </si>
+  <si>
+    <t>Rear Corner 2</t>
+  </si>
+  <si>
+    <t>Rear Wall</t>
+  </si>
+  <si>
+    <t>00000010</t>
+  </si>
+  <si>
+    <t>Left R Corner 1</t>
+  </si>
+  <si>
+    <t>Left R Corner 2</t>
+  </si>
+  <si>
+    <t>Left R Corner 3</t>
+  </si>
+  <si>
+    <t>Left R Corner 4</t>
+  </si>
+  <si>
+    <t>00000011</t>
   </si>
 </sst>
 </file>
@@ -428,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -445,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -453,110 +510,198 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>10000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
-        <v>11100</v>
+        <v>11100000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
-        <v>11000</v>
+        <v>11000000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
-        <v>10100</v>
+        <v>10100000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>10000011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>10000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24">
+        <v>10000010</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B6:B14" numberStoredAsText="1"/>
+    <ignoredError sqref="B5:B25" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>